<commit_message>
Mise à jour du gantt
</commit_message>
<xml_diff>
--- a/Diagramme de Gantt.xlsx
+++ b/Diagramme de Gantt.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
   <si>
     <t xml:space="preserve">MODÈLE DE DIAGRAMME DE GANTT</t>
   </si>
@@ -162,34 +162,49 @@
     <t xml:space="preserve">Réalisation du cahier des charges</t>
   </si>
   <si>
+    <t xml:space="preserve">Analyse Algorithmique de la version 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analyse Algorithmique de la version finale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Codage &amp; Test </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Récupération d’un projet existant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">’3.1.1 ‘</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test du code Existant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soumia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'3.1.2’</t>
+  </si>
+  <si>
     <t xml:space="preserve">Réalisation d’un Makefile générique</t>
   </si>
   <si>
     <t xml:space="preserve">Xavier</t>
   </si>
   <si>
-    <t xml:space="preserve">Codage &amp; Test </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Récupération d’un projet existant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">’3.1.1 ‘</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test du code Existant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soumia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'3.1.2’</t>
-  </si>
-  <si>
     <t xml:space="preserve">3.2.2</t>
   </si>
   <si>
     <t xml:space="preserve">3.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contrôle du projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Préparation du rapport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Préparation de la soutenance</t>
   </si>
 </sst>
 </file>
@@ -1169,15 +1184,15 @@
   </sheetPr>
   <dimension ref="A1:BQ36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB20" activeCellId="0" sqref="AB20"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="34.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.63"/>
@@ -2347,7 +2362,7 @@
         <v>13</v>
       </c>
       <c r="H14" s="58" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="68"/>
       <c r="J14" s="69"/>
@@ -2432,7 +2447,9 @@
         <f aca="false">DAYS360(E15,F15)</f>
         <v>24</v>
       </c>
-      <c r="H15" s="58"/>
+      <c r="H15" s="58" t="n">
+        <v>0.5</v>
+      </c>
       <c r="I15" s="68"/>
       <c r="J15" s="69"/>
       <c r="K15" s="70"/>
@@ -2517,7 +2534,7 @@
         <v>2</v>
       </c>
       <c r="H16" s="80" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="I16" s="68"/>
       <c r="J16" s="69"/>
@@ -2747,25 +2764,8 @@
       <c r="B19" s="54" t="n">
         <v>43133</v>
       </c>
-      <c r="C19" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="56" t="n">
-        <v>44966</v>
-      </c>
-      <c r="F19" s="56" t="n">
-        <v>44966</v>
-      </c>
-      <c r="G19" s="57" t="n">
-        <f aca="false">DAYS360(E19,F19)</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="58" t="n">
-        <v>1</v>
-      </c>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
       <c r="I19" s="68"/>
       <c r="J19" s="69"/>
       <c r="K19" s="70"/>
@@ -2833,8 +2833,12 @@
       <c r="B20" s="54" t="n">
         <v>43161</v>
       </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
+      <c r="C20" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="55" t="s">
+        <v>37</v>
+      </c>
       <c r="E20" s="56"/>
       <c r="F20" s="56"/>
       <c r="G20" s="57" t="n">
@@ -2842,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="58" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="I20" s="68"/>
       <c r="J20" s="69"/>
@@ -2911,8 +2915,12 @@
       <c r="B21" s="54" t="n">
         <v>43192</v>
       </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
+      <c r="C21" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>37</v>
+      </c>
       <c r="E21" s="56"/>
       <c r="F21" s="56"/>
       <c r="G21" s="57" t="n">
@@ -3159,13 +3167,15 @@
       <c r="E24" s="56" t="n">
         <v>44966</v>
       </c>
-      <c r="F24" s="56"/>
+      <c r="F24" s="56" t="n">
+        <v>44988</v>
+      </c>
       <c r="G24" s="57" t="n">
         <f aca="false">DAYS360(E24,F24)</f>
-        <v>-44319</v>
+        <v>24</v>
       </c>
       <c r="H24" s="58" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="I24" s="68"/>
       <c r="J24" s="69"/>
@@ -3234,10 +3244,24 @@
       <c r="B25" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="0"/>
-      <c r="D25" s="0"/>
+      <c r="C25" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="56" t="n">
+        <v>44966</v>
+      </c>
+      <c r="F25" s="56" t="n">
+        <v>44966</v>
+      </c>
+      <c r="G25" s="57" t="n">
+        <f aca="false">DAYS360(E25,F25)</f>
+        <v>0</v>
+      </c>
       <c r="H25" s="58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="68"/>
       <c r="J25" s="69"/>
@@ -3304,7 +3328,7 @@
     <row r="26" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A26" s="53"/>
       <c r="B26" s="67" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C26" s="55"/>
       <c r="D26" s="55"/>
@@ -3460,7 +3484,7 @@
     <row r="28" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A28" s="53"/>
       <c r="B28" s="67" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C28" s="55"/>
       <c r="D28" s="55"/>
@@ -3540,7 +3564,9 @@
       <c r="B29" s="47" t="n">
         <v>4</v>
       </c>
-      <c r="C29" s="48"/>
+      <c r="C29" s="48" t="s">
+        <v>58</v>
+      </c>
       <c r="D29" s="48"/>
       <c r="E29" s="49"/>
       <c r="F29" s="49"/>
@@ -3613,8 +3639,12 @@
       <c r="B30" s="54" t="n">
         <v>43104</v>
       </c>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
+      <c r="C30" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="55" t="s">
+        <v>37</v>
+      </c>
       <c r="E30" s="56"/>
       <c r="F30" s="56"/>
       <c r="G30" s="57" t="n">
@@ -3691,8 +3721,12 @@
       <c r="B31" s="54" t="n">
         <v>43135</v>
       </c>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
+      <c r="C31" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="55" t="s">
+        <v>37</v>
+      </c>
       <c r="E31" s="56"/>
       <c r="F31" s="56"/>
       <c r="G31" s="57" t="n">
@@ -4170,7 +4204,7 @@
     <mergeCell ref="BG9:BK9"/>
     <mergeCell ref="BL9:BP9"/>
   </mergeCells>
-  <conditionalFormatting sqref="H12:H16 H18:H33">
+  <conditionalFormatting sqref="H12:H16 H26:H33 H18 H20:H24">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4180,7 +4214,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H16 H18:H33">
+  <conditionalFormatting sqref="H12:H16 H26:H33 H18 H20:H24">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4250,6 +4284,26 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FF57BB8A"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF57BB8A"/>
+        <color rgb="FFFFFFFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>